<commit_message>
Splitting the GO into new file
</commit_message>
<xml_diff>
--- a/Results/GO_DMGenes_woUPDOWN_0.01.xlsx
+++ b/Results/GO_DMGenes_woUPDOWN_0.01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19392" windowHeight="9168"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19392" windowHeight="9168" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="K4hU" sheetId="1" r:id="rId1"/>
@@ -2237,18 +2237,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2268,6 +2262,60 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2281,12 +2329,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2569,8 +2625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2610,7 +2666,7 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C2">
@@ -2636,7 +2692,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C3">
@@ -2688,7 +2744,7 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C5">
@@ -2740,7 +2796,7 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C7">
@@ -2818,7 +2874,7 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C10">
@@ -2844,7 +2900,7 @@
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C11">
@@ -2870,7 +2926,7 @@
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C12">
@@ -2922,7 +2978,7 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C14">
@@ -2974,7 +3030,7 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C16">
@@ -3052,7 +3108,7 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C19">
@@ -3078,7 +3134,7 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C20">
@@ -3182,7 +3238,7 @@
       <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C24">
@@ -3208,7 +3264,7 @@
       <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C25">
@@ -3234,7 +3290,7 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C26">
@@ -3260,7 +3316,7 @@
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C27">
@@ -3312,7 +3368,7 @@
       <c r="A29" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C29">
@@ -3338,7 +3394,7 @@
       <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C30">
@@ -3364,7 +3420,7 @@
       <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C31">
@@ -3390,7 +3446,7 @@
       <c r="A32" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C32">
@@ -3520,7 +3576,7 @@
       <c r="A37" t="s">
         <v>43</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C37">
@@ -3598,7 +3654,7 @@
       <c r="A40" t="s">
         <v>46</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>140</v>
       </c>
       <c r="C40">
@@ -3676,7 +3732,7 @@
       <c r="A43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="6" t="s">
         <v>143</v>
       </c>
       <c r="C43">
@@ -3728,7 +3784,7 @@
       <c r="A45" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C45">
@@ -3806,7 +3862,7 @@
       <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C48">
@@ -3858,7 +3914,7 @@
       <c r="A50" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>150</v>
       </c>
       <c r="C50">
@@ -3884,7 +3940,7 @@
       <c r="A51" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C51">
@@ -3910,7 +3966,7 @@
       <c r="A52" t="s">
         <v>58</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="6" t="s">
         <v>152</v>
       </c>
       <c r="C52">
@@ -3936,7 +3992,7 @@
       <c r="A53" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>153</v>
       </c>
       <c r="C53">
@@ -4014,7 +4070,7 @@
       <c r="A56" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C56">
@@ -4196,7 +4252,7 @@
       <c r="A63" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C63">
@@ -4248,7 +4304,7 @@
       <c r="A65" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>165</v>
       </c>
       <c r="C65">
@@ -4300,7 +4356,7 @@
       <c r="A67" t="s">
         <v>73</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C67">
@@ -4352,7 +4408,7 @@
       <c r="A69" t="s">
         <v>75</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="6" t="s">
         <v>169</v>
       </c>
       <c r="C69">
@@ -4378,7 +4434,7 @@
       <c r="A70" t="s">
         <v>76</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C70">
@@ -4456,7 +4512,7 @@
       <c r="A73" t="s">
         <v>79</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>173</v>
       </c>
       <c r="C73">
@@ -4534,7 +4590,7 @@
       <c r="A76" t="s">
         <v>82</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="6" t="s">
         <v>176</v>
       </c>
       <c r="C76">
@@ -4560,7 +4616,7 @@
       <c r="A77" t="s">
         <v>83</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C77">
@@ -4612,7 +4668,7 @@
       <c r="A79" t="s">
         <v>85</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C79">
@@ -4638,7 +4694,7 @@
       <c r="A80" t="s">
         <v>86</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C80">
@@ -4664,7 +4720,7 @@
       <c r="A81" t="s">
         <v>87</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C81">
@@ -4690,7 +4746,7 @@
       <c r="A82" t="s">
         <v>88</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="4" t="s">
         <v>182</v>
       </c>
       <c r="C82">
@@ -4716,7 +4772,7 @@
       <c r="A83" t="s">
         <v>89</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="4" t="s">
         <v>183</v>
       </c>
       <c r="C83">
@@ -4820,7 +4876,7 @@
       <c r="A87" t="s">
         <v>93</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C87">
@@ -4872,7 +4928,7 @@
       <c r="A89" t="s">
         <v>95</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="5" t="s">
         <v>189</v>
       </c>
       <c r="C89">
@@ -4976,7 +5032,7 @@
       <c r="A93" t="s">
         <v>99</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="6" t="s">
         <v>193</v>
       </c>
       <c r="C93">
@@ -5028,7 +5084,7 @@
       <c r="A95" t="s">
         <v>101</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="6" t="s">
         <v>195</v>
       </c>
       <c r="C95">
@@ -5059,9 +5115,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5119,7 +5180,7 @@
       <c r="A3" t="s">
         <v>197</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C3">
@@ -5145,7 +5206,7 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C4">
@@ -5197,7 +5258,7 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C6">
@@ -5249,7 +5310,7 @@
       <c r="A8" t="s">
         <v>199</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>284</v>
       </c>
       <c r="C8">
@@ -5275,7 +5336,7 @@
       <c r="A9" t="s">
         <v>200</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>285</v>
       </c>
       <c r="C9">
@@ -5301,7 +5362,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C10">
@@ -5353,7 +5414,7 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C12">
@@ -5431,7 +5492,7 @@
       <c r="A15" t="s">
         <v>204</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>289</v>
       </c>
       <c r="C15">
@@ -5483,7 +5544,7 @@
       <c r="A17" t="s">
         <v>205</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>290</v>
       </c>
       <c r="C17">
@@ -5535,7 +5596,7 @@
       <c r="A19" t="s">
         <v>206</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>291</v>
       </c>
       <c r="C19">
@@ -5639,7 +5700,7 @@
       <c r="A23" t="s">
         <v>210</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>295</v>
       </c>
       <c r="C23">
@@ -5665,7 +5726,7 @@
       <c r="A24" t="s">
         <v>211</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C24">
@@ -5691,7 +5752,7 @@
       <c r="A25" t="s">
         <v>212</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>297</v>
       </c>
       <c r="C25">
@@ -5717,7 +5778,7 @@
       <c r="A26" t="s">
         <v>213</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>298</v>
       </c>
       <c r="C26">
@@ -5743,7 +5804,7 @@
       <c r="A27" t="s">
         <v>214</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>299</v>
       </c>
       <c r="C27">
@@ -5821,7 +5882,7 @@
       <c r="A30" t="s">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>165</v>
       </c>
       <c r="C30">
@@ -5847,7 +5908,7 @@
       <c r="A31" t="s">
         <v>217</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>302</v>
       </c>
       <c r="C31">
@@ -5899,7 +5960,7 @@
       <c r="A33" t="s">
         <v>219</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>304</v>
       </c>
       <c r="C33">
@@ -6029,7 +6090,7 @@
       <c r="A38" t="s">
         <v>224</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="7" t="s">
         <v>309</v>
       </c>
       <c r="C38">
@@ -6341,7 +6402,7 @@
       <c r="A50" t="s">
         <v>39</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C50">
@@ -6419,7 +6480,7 @@
       <c r="A53" t="s">
         <v>238</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="8" t="s">
         <v>323</v>
       </c>
       <c r="C53">
@@ -6471,7 +6532,7 @@
       <c r="A55" t="s">
         <v>240</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="8" t="s">
         <v>325</v>
       </c>
       <c r="C55">
@@ -6497,7 +6558,7 @@
       <c r="A56" t="s">
         <v>241</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>326</v>
       </c>
       <c r="C56">
@@ -6523,7 +6584,7 @@
       <c r="A57" t="s">
         <v>242</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="6" t="s">
         <v>327</v>
       </c>
       <c r="C57">
@@ -6575,7 +6636,7 @@
       <c r="A59" t="s">
         <v>244</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>329</v>
       </c>
       <c r="C59">
@@ -6653,7 +6714,7 @@
       <c r="A62" t="s">
         <v>246</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="6" t="s">
         <v>331</v>
       </c>
       <c r="C62">
@@ -6679,7 +6740,7 @@
       <c r="A63" t="s">
         <v>247</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>332</v>
       </c>
       <c r="C63">
@@ -6783,7 +6844,7 @@
       <c r="A67" t="s">
         <v>250</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="8" t="s">
         <v>335</v>
       </c>
       <c r="C67">
@@ -6939,7 +7000,7 @@
       <c r="A73" t="s">
         <v>254</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="6" t="s">
         <v>339</v>
       </c>
       <c r="C73">
@@ -6965,7 +7026,7 @@
       <c r="A74" t="s">
         <v>255</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>340</v>
       </c>
       <c r="C74">
@@ -7017,7 +7078,7 @@
       <c r="A76" t="s">
         <v>257</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="12" t="s">
         <v>342</v>
       </c>
       <c r="C76">
@@ -7043,7 +7104,7 @@
       <c r="A77" t="s">
         <v>258</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C77">
@@ -7069,7 +7130,7 @@
       <c r="A78" t="s">
         <v>259</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="12" t="s">
         <v>344</v>
       </c>
       <c r="C78">
@@ -7147,7 +7208,7 @@
       <c r="A81" t="s">
         <v>262</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>347</v>
       </c>
       <c r="C81">
@@ -7173,7 +7234,7 @@
       <c r="A82" t="s">
         <v>263</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>348</v>
       </c>
       <c r="C82">
@@ -7199,7 +7260,7 @@
       <c r="A83" t="s">
         <v>264</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="12" t="s">
         <v>349</v>
       </c>
       <c r="C83">
@@ -7225,7 +7286,7 @@
       <c r="A84" t="s">
         <v>265</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="12" t="s">
         <v>350</v>
       </c>
       <c r="C84">
@@ -7381,7 +7442,7 @@
       <c r="A90" t="s">
         <v>17</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C90">
@@ -7459,7 +7520,7 @@
       <c r="A93" t="s">
         <v>273</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="5" t="s">
         <v>358</v>
       </c>
       <c r="C93">
@@ -7485,7 +7546,7 @@
       <c r="A94" t="s">
         <v>274</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="12" t="s">
         <v>359</v>
       </c>
       <c r="C94">
@@ -7537,7 +7598,7 @@
       <c r="A96" t="s">
         <v>276</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>361</v>
       </c>
       <c r="C96">
@@ -7589,7 +7650,7 @@
       <c r="A98" t="s">
         <v>278</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="5" t="s">
         <v>363</v>
       </c>
       <c r="C98">
@@ -7615,7 +7676,7 @@
       <c r="A99" t="s">
         <v>279</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="12" t="s">
         <v>364</v>
       </c>
       <c r="C99">
@@ -7672,9 +7733,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="50.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7758,7 +7824,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C4">
@@ -7784,7 +7850,7 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C5">
@@ -7810,7 +7876,7 @@
       <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>173</v>
       </c>
       <c r="C6">
@@ -7836,7 +7902,7 @@
       <c r="A7" t="s">
         <v>244</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>329</v>
       </c>
       <c r="C7">
@@ -7862,7 +7928,7 @@
       <c r="A8" t="s">
         <v>210</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>295</v>
       </c>
       <c r="C8">
@@ -7888,7 +7954,7 @@
       <c r="A9" t="s">
         <v>366</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>432</v>
       </c>
       <c r="C9">
@@ -7914,7 +7980,7 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>112</v>
       </c>
       <c r="C10">
@@ -7966,7 +8032,7 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>102</v>
       </c>
       <c r="C12">
@@ -7992,7 +8058,7 @@
       <c r="A13" t="s">
         <v>367</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>433</v>
       </c>
       <c r="C13">
@@ -8044,7 +8110,7 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C15">
@@ -8070,7 +8136,7 @@
       <c r="A16" t="s">
         <v>71</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>165</v>
       </c>
       <c r="C16">
@@ -8096,7 +8162,7 @@
       <c r="A17" t="s">
         <v>369</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>435</v>
       </c>
       <c r="C17">
@@ -8148,7 +8214,7 @@
       <c r="A19" t="s">
         <v>370</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>436</v>
       </c>
       <c r="C19">
@@ -8174,7 +8240,7 @@
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C20">
@@ -8226,7 +8292,7 @@
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C22">
@@ -8278,7 +8344,7 @@
       <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C24">
@@ -8304,7 +8370,7 @@
       <c r="A25" t="s">
         <v>373</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>439</v>
       </c>
       <c r="C25">
@@ -8330,7 +8396,7 @@
       <c r="A26" t="s">
         <v>95</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>189</v>
       </c>
       <c r="C26">
@@ -8486,7 +8552,7 @@
       <c r="A32" t="s">
         <v>377</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>443</v>
       </c>
       <c r="C32">
@@ -8538,7 +8604,7 @@
       <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C34">
@@ -8564,7 +8630,7 @@
       <c r="A35" t="s">
         <v>241</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>326</v>
       </c>
       <c r="C35">
@@ -8590,7 +8656,7 @@
       <c r="A36" t="s">
         <v>379</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>445</v>
       </c>
       <c r="C36">
@@ -8668,7 +8734,7 @@
       <c r="A39" t="s">
         <v>382</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>448</v>
       </c>
       <c r="C39">
@@ -8694,7 +8760,7 @@
       <c r="A40" t="s">
         <v>383</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>449</v>
       </c>
       <c r="C40">
@@ -8720,7 +8786,7 @@
       <c r="A41" t="s">
         <v>384</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>450</v>
       </c>
       <c r="C41">
@@ -8772,7 +8838,7 @@
       <c r="A43" t="s">
         <v>58</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="6" t="s">
         <v>152</v>
       </c>
       <c r="C43">
@@ -8824,7 +8890,7 @@
       <c r="A45" t="s">
         <v>386</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>452</v>
       </c>
       <c r="C45">
@@ -8928,7 +8994,7 @@
       <c r="A49" t="s">
         <v>390</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>456</v>
       </c>
       <c r="C49">
@@ -8954,7 +9020,7 @@
       <c r="A50" t="s">
         <v>75</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="6" t="s">
         <v>169</v>
       </c>
       <c r="C50">
@@ -8980,7 +9046,7 @@
       <c r="A51" t="s">
         <v>391</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>457</v>
       </c>
       <c r="C51">
@@ -9136,7 +9202,7 @@
       <c r="A57" t="s">
         <v>395</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>461</v>
       </c>
       <c r="C57">
@@ -9162,7 +9228,7 @@
       <c r="A58" t="s">
         <v>43</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C58">
@@ -9188,7 +9254,7 @@
       <c r="A59" t="s">
         <v>396</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="10" t="s">
         <v>462</v>
       </c>
       <c r="C59">
@@ -9214,7 +9280,7 @@
       <c r="A60" t="s">
         <v>397</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C60">
@@ -9240,7 +9306,7 @@
       <c r="A61" t="s">
         <v>197</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="10" t="s">
         <v>282</v>
       </c>
       <c r="C61">
@@ -9266,7 +9332,7 @@
       <c r="A62" t="s">
         <v>49</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="10" t="s">
         <v>143</v>
       </c>
       <c r="C62">
@@ -9292,7 +9358,7 @@
       <c r="A63" t="s">
         <v>398</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>464</v>
       </c>
       <c r="C63">
@@ -9318,7 +9384,7 @@
       <c r="A64" t="s">
         <v>399</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="10" t="s">
         <v>465</v>
       </c>
       <c r="C64">
@@ -9370,7 +9436,7 @@
       <c r="A66" t="s">
         <v>400</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>466</v>
       </c>
       <c r="C66">
@@ -9396,7 +9462,7 @@
       <c r="A67" t="s">
         <v>86</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C67">
@@ -9422,7 +9488,7 @@
       <c r="A68" t="s">
         <v>238</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="8" t="s">
         <v>323</v>
       </c>
       <c r="C68">
@@ -9552,7 +9618,7 @@
       <c r="A73" t="s">
         <v>404</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C73">
@@ -9578,7 +9644,7 @@
       <c r="A74" t="s">
         <v>405</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>471</v>
       </c>
       <c r="C74">
@@ -9604,7 +9670,7 @@
       <c r="A75" t="s">
         <v>57</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C75">
@@ -9708,7 +9774,7 @@
       <c r="A79" t="s">
         <v>407</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="3" t="s">
         <v>473</v>
       </c>
       <c r="C79">
@@ -9734,7 +9800,7 @@
       <c r="A80" t="s">
         <v>56</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="3" t="s">
         <v>150</v>
       </c>
       <c r="C80">
@@ -9760,7 +9826,7 @@
       <c r="A81" t="s">
         <v>408</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="3" t="s">
         <v>474</v>
       </c>
       <c r="C81">
@@ -9786,7 +9852,7 @@
       <c r="A82" t="s">
         <v>26</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C82">
@@ -9838,7 +9904,7 @@
       <c r="A84" t="s">
         <v>59</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="3" t="s">
         <v>153</v>
       </c>
       <c r="C84">
@@ -9864,7 +9930,7 @@
       <c r="A85" t="s">
         <v>410</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>476</v>
       </c>
       <c r="C85">
@@ -9916,7 +9982,7 @@
       <c r="A87" t="s">
         <v>412</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>478</v>
       </c>
       <c r="C87">
@@ -9942,7 +10008,7 @@
       <c r="A88" t="s">
         <v>413</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="4" t="s">
         <v>479</v>
       </c>
       <c r="C88">
@@ -9968,7 +10034,7 @@
       <c r="A89" t="s">
         <v>414</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="4" t="s">
         <v>480</v>
       </c>
       <c r="C89">
@@ -10176,7 +10242,7 @@
       <c r="A97" t="s">
         <v>421</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="10" t="s">
         <v>487</v>
       </c>
       <c r="C97">
@@ -10228,7 +10294,7 @@
       <c r="A99" t="s">
         <v>224</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="3" t="s">
         <v>309</v>
       </c>
       <c r="C99">
@@ -10254,7 +10320,7 @@
       <c r="A100" t="s">
         <v>22</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C100">
@@ -10306,7 +10372,7 @@
       <c r="A102" t="s">
         <v>422</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="6" t="s">
         <v>488</v>
       </c>
       <c r="C102">
@@ -10436,7 +10502,7 @@
       <c r="A107" t="s">
         <v>426</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="6" t="s">
         <v>492</v>
       </c>
       <c r="C107">
@@ -10514,7 +10580,7 @@
       <c r="A110" t="s">
         <v>427</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="6" t="s">
         <v>493</v>
       </c>
       <c r="C110">
@@ -10540,7 +10606,7 @@
       <c r="A111" t="s">
         <v>87</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C111">
@@ -10592,7 +10658,7 @@
       <c r="A113" t="s">
         <v>93</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C113">
@@ -10618,7 +10684,7 @@
       <c r="A114" t="s">
         <v>205</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C114">
@@ -10644,7 +10710,7 @@
       <c r="A115" t="s">
         <v>429</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="9" t="s">
         <v>495</v>
       </c>
       <c r="C115">
@@ -10670,7 +10736,7 @@
       <c r="A116" t="s">
         <v>430</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="3" t="s">
         <v>496</v>
       </c>
       <c r="C116">
@@ -10753,9 +10819,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10787,7 +10858,7 @@
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C2">
@@ -10813,7 +10884,7 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C3">
@@ -10839,7 +10910,7 @@
       <c r="A4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>152</v>
       </c>
       <c r="C4">
@@ -10891,7 +10962,7 @@
       <c r="A6" t="s">
         <v>498</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>526</v>
       </c>
       <c r="C6">
@@ -10943,7 +11014,7 @@
       <c r="A8" t="s">
         <v>500</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>528</v>
       </c>
       <c r="C8">
@@ -10995,7 +11066,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C10">
@@ -11021,7 +11092,7 @@
       <c r="A11" t="s">
         <v>502</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>530</v>
       </c>
       <c r="C11">
@@ -11047,7 +11118,7 @@
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C12">
@@ -11073,7 +11144,7 @@
       <c r="A13" t="s">
         <v>503</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>531</v>
       </c>
       <c r="C13">
@@ -11125,7 +11196,7 @@
       <c r="A15" t="s">
         <v>504</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="12" t="s">
         <v>532</v>
       </c>
       <c r="C15">
@@ -11203,7 +11274,7 @@
       <c r="A18" t="s">
         <v>506</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>534</v>
       </c>
       <c r="C18">
@@ -11229,7 +11300,7 @@
       <c r="A19" t="s">
         <v>224</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>309</v>
       </c>
       <c r="C19">
@@ -11255,7 +11326,7 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C20">
@@ -11281,7 +11352,7 @@
       <c r="A21" t="s">
         <v>507</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>535</v>
       </c>
       <c r="C21">
@@ -11307,7 +11378,7 @@
       <c r="A22" t="s">
         <v>272</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>357</v>
       </c>
       <c r="C22">
@@ -11333,7 +11404,7 @@
       <c r="A23" t="s">
         <v>508</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>536</v>
       </c>
       <c r="C23">
@@ -11411,7 +11482,7 @@
       <c r="A26" t="s">
         <v>407</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>473</v>
       </c>
       <c r="C26">
@@ -11463,7 +11534,7 @@
       <c r="A28" t="s">
         <v>512</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>540</v>
       </c>
       <c r="C28">
@@ -11489,7 +11560,7 @@
       <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>119</v>
       </c>
       <c r="C29">
@@ -11541,7 +11612,7 @@
       <c r="A31" t="s">
         <v>514</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>542</v>
       </c>
       <c r="C31">
@@ -11567,7 +11638,7 @@
       <c r="A32" t="s">
         <v>515</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>543</v>
       </c>
       <c r="C32">
@@ -11593,7 +11664,7 @@
       <c r="A33" t="s">
         <v>101</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>195</v>
       </c>
       <c r="C33">
@@ -11619,7 +11690,7 @@
       <c r="A34" t="s">
         <v>516</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>544</v>
       </c>
       <c r="C34">
@@ -11671,7 +11742,7 @@
       <c r="A36" t="s">
         <v>518</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>546</v>
       </c>
       <c r="C36">
@@ -11801,7 +11872,7 @@
       <c r="A41" t="s">
         <v>522</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>550</v>
       </c>
       <c r="C41">
@@ -11827,7 +11898,7 @@
       <c r="A42" t="s">
         <v>523</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>551</v>
       </c>
       <c r="C42">
@@ -11853,7 +11924,7 @@
       <c r="A43" t="s">
         <v>524</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="6" t="s">
         <v>552</v>
       </c>
       <c r="C43">
@@ -11936,9 +12007,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B55" activeCellId="1" sqref="B60 B55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -11970,7 +12046,7 @@
       <c r="A2" t="s">
         <v>244</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>329</v>
       </c>
       <c r="C2">
@@ -11996,7 +12072,7 @@
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>189</v>
       </c>
       <c r="C3">
@@ -12048,7 +12124,7 @@
       <c r="A5" t="s">
         <v>555</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>613</v>
       </c>
       <c r="C5">
@@ -12100,7 +12176,7 @@
       <c r="A7" t="s">
         <v>557</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>615</v>
       </c>
       <c r="C7">
@@ -12126,7 +12202,7 @@
       <c r="A8" t="s">
         <v>558</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>616</v>
       </c>
       <c r="C8">
@@ -12152,7 +12228,7 @@
       <c r="A9" t="s">
         <v>559</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>617</v>
       </c>
       <c r="C9">
@@ -12178,7 +12254,7 @@
       <c r="A10" t="s">
         <v>560</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>618</v>
       </c>
       <c r="C10">
@@ -12230,7 +12306,7 @@
       <c r="A12" t="s">
         <v>562</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>620</v>
       </c>
       <c r="C12">
@@ -12256,7 +12332,7 @@
       <c r="A13" t="s">
         <v>563</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>621</v>
       </c>
       <c r="C13">
@@ -12282,7 +12358,7 @@
       <c r="A14" t="s">
         <v>564</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>622</v>
       </c>
       <c r="C14">
@@ -12308,7 +12384,7 @@
       <c r="A15" t="s">
         <v>565</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>623</v>
       </c>
       <c r="C15">
@@ -12334,7 +12410,7 @@
       <c r="A16" t="s">
         <v>566</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="12" t="s">
         <v>624</v>
       </c>
       <c r="C16">
@@ -12464,7 +12540,7 @@
       <c r="A21" t="s">
         <v>571</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="10" t="s">
         <v>629</v>
       </c>
       <c r="C21">
@@ -12490,7 +12566,7 @@
       <c r="A22" t="s">
         <v>572</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>630</v>
       </c>
       <c r="C22">
@@ -12568,7 +12644,7 @@
       <c r="A25" t="s">
         <v>575</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>633</v>
       </c>
       <c r="C25">
@@ -12620,7 +12696,7 @@
       <c r="A27" t="s">
         <v>577</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>635</v>
       </c>
       <c r="C27">
@@ -12646,7 +12722,7 @@
       <c r="A28" t="s">
         <v>578</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>636</v>
       </c>
       <c r="C28">
@@ -12672,7 +12748,7 @@
       <c r="A29" t="s">
         <v>579</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="10" t="s">
         <v>637</v>
       </c>
       <c r="C29">
@@ -12698,7 +12774,7 @@
       <c r="A30" t="s">
         <v>580</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="10" t="s">
         <v>638</v>
       </c>
       <c r="C30">
@@ -12776,7 +12852,7 @@
       <c r="A33" t="s">
         <v>583</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>641</v>
       </c>
       <c r="C33">
@@ -12802,7 +12878,7 @@
       <c r="A34" t="s">
         <v>584</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="10" t="s">
         <v>642</v>
       </c>
       <c r="C34">
@@ -12828,7 +12904,7 @@
       <c r="A35" t="s">
         <v>585</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="10" t="s">
         <v>643</v>
       </c>
       <c r="C35">
@@ -12906,7 +12982,7 @@
       <c r="A38" t="s">
         <v>588</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="10" t="s">
         <v>646</v>
       </c>
       <c r="C38">
@@ -12958,7 +13034,7 @@
       <c r="A40" t="s">
         <v>590</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="10" t="s">
         <v>648</v>
       </c>
       <c r="C40">
@@ -13036,7 +13112,7 @@
       <c r="A43" t="s">
         <v>593</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="10" t="s">
         <v>651</v>
       </c>
       <c r="C43">
@@ -13088,7 +13164,7 @@
       <c r="A45" t="s">
         <v>595</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="10" t="s">
         <v>653</v>
       </c>
       <c r="C45">
@@ -13140,7 +13216,7 @@
       <c r="A47" t="s">
         <v>597</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="10" t="s">
         <v>655</v>
       </c>
       <c r="C47">
@@ -13192,7 +13268,7 @@
       <c r="A49" t="s">
         <v>599</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="10" t="s">
         <v>657</v>
       </c>
       <c r="C49">
@@ -13218,7 +13294,7 @@
       <c r="A50" t="s">
         <v>600</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="10" t="s">
         <v>658</v>
       </c>
       <c r="C50">
@@ -13322,7 +13398,7 @@
       <c r="A54" t="s">
         <v>604</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="10" t="s">
         <v>662</v>
       </c>
       <c r="C54">
@@ -13348,7 +13424,7 @@
       <c r="A55" t="s">
         <v>605</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="11" t="s">
         <v>663</v>
       </c>
       <c r="C55">
@@ -13374,7 +13450,7 @@
       <c r="A56" t="s">
         <v>606</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="10" t="s">
         <v>664</v>
       </c>
       <c r="C56">
@@ -13400,7 +13476,7 @@
       <c r="A57" t="s">
         <v>607</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="10" t="s">
         <v>665</v>
       </c>
       <c r="C57">
@@ -13426,7 +13502,7 @@
       <c r="A58" t="s">
         <v>608</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>666</v>
       </c>
       <c r="C58">
@@ -13478,7 +13554,7 @@
       <c r="A60" t="s">
         <v>610</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="11" t="s">
         <v>668</v>
       </c>
       <c r="C60">
@@ -13528,6 +13604,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13535,9 +13612,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="52.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13621,7 +13703,7 @@
       <c r="A4" t="s">
         <v>672</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>678</v>
       </c>
       <c r="C4">
@@ -13756,9 +13838,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13790,7 +13877,7 @@
       <c r="A2" t="s">
         <v>244</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>329</v>
       </c>
       <c r="C2">
@@ -13816,7 +13903,7 @@
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>189</v>
       </c>
       <c r="C3">
@@ -13842,7 +13929,7 @@
       <c r="A4" t="s">
         <v>555</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>613</v>
       </c>
       <c r="C4">
@@ -13894,7 +13981,7 @@
       <c r="A6" t="s">
         <v>575</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>633</v>
       </c>
       <c r="C6">
@@ -14050,7 +14137,7 @@
       <c r="A12" t="s">
         <v>566</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="12" t="s">
         <v>624</v>
       </c>
       <c r="C12">
@@ -14102,7 +14189,7 @@
       <c r="A14" t="s">
         <v>558</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="10" t="s">
         <v>616</v>
       </c>
       <c r="C14">
@@ -14128,7 +14215,7 @@
       <c r="A15" t="s">
         <v>580</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>638</v>
       </c>
       <c r="C15">
@@ -14154,7 +14241,7 @@
       <c r="A16" t="s">
         <v>557</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
         <v>615</v>
       </c>
       <c r="C16">
@@ -14180,7 +14267,7 @@
       <c r="A17" t="s">
         <v>572</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="10" t="s">
         <v>630</v>
       </c>
       <c r="C17">
@@ -14206,7 +14293,7 @@
       <c r="A18" t="s">
         <v>599</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="10" t="s">
         <v>657</v>
       </c>
       <c r="C18">
@@ -14232,7 +14319,7 @@
       <c r="A19" t="s">
         <v>683</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>700</v>
       </c>
       <c r="C19">
@@ -14258,7 +14345,7 @@
       <c r="A20" t="s">
         <v>559</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="10" t="s">
         <v>617</v>
       </c>
       <c r="C20">
@@ -14310,7 +14397,7 @@
       <c r="A22" t="s">
         <v>565</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>623</v>
       </c>
       <c r="C22">
@@ -14336,7 +14423,7 @@
       <c r="A23" t="s">
         <v>562</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="10" t="s">
         <v>620</v>
       </c>
       <c r="C23">
@@ -14466,7 +14553,7 @@
       <c r="A28" t="s">
         <v>571</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>629</v>
       </c>
       <c r="C28">
@@ -14492,7 +14579,7 @@
       <c r="A29" t="s">
         <v>684</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="10" t="s">
         <v>701</v>
       </c>
       <c r="C29">
@@ -14518,7 +14605,7 @@
       <c r="A30" t="s">
         <v>685</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>702</v>
       </c>
       <c r="C30">
@@ -14544,7 +14631,7 @@
       <c r="A31" t="s">
         <v>577</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="10" t="s">
         <v>635</v>
       </c>
       <c r="C31">
@@ -14570,7 +14657,7 @@
       <c r="A32" t="s">
         <v>686</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="10" t="s">
         <v>703</v>
       </c>
       <c r="C32">
@@ -14622,7 +14709,7 @@
       <c r="A34" t="s">
         <v>687</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="10" t="s">
         <v>704</v>
       </c>
       <c r="C34">
@@ -14648,7 +14735,7 @@
       <c r="A35" t="s">
         <v>564</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>622</v>
       </c>
       <c r="C35">
@@ -14700,7 +14787,7 @@
       <c r="A37" t="s">
         <v>563</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="10" t="s">
         <v>621</v>
       </c>
       <c r="C37">
@@ -14778,7 +14865,7 @@
       <c r="A40" t="s">
         <v>608</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>666</v>
       </c>
       <c r="C40">
@@ -14830,7 +14917,7 @@
       <c r="A42" t="s">
         <v>690</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="10" t="s">
         <v>707</v>
       </c>
       <c r="C42">
@@ -14856,7 +14943,7 @@
       <c r="A43" t="s">
         <v>560</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="10" t="s">
         <v>618</v>
       </c>
       <c r="C43">
@@ -14908,7 +14995,7 @@
       <c r="A45" t="s">
         <v>692</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="10" t="s">
         <v>709</v>
       </c>
       <c r="C45">
@@ -14934,7 +15021,7 @@
       <c r="A46" t="s">
         <v>693</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="10" t="s">
         <v>710</v>
       </c>
       <c r="C46">
@@ -14960,7 +15047,7 @@
       <c r="A47" t="s">
         <v>694</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="10" t="s">
         <v>711</v>
       </c>
       <c r="C47">
@@ -15064,7 +15151,7 @@
       <c r="A51" t="s">
         <v>698</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="10" t="s">
         <v>715</v>
       </c>
       <c r="C51">
@@ -15121,9 +15208,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -15285,7 +15377,7 @@
       <c r="A7" t="s">
         <v>720</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>728</v>
       </c>
       <c r="C7">
@@ -15311,7 +15403,7 @@
       <c r="A8" t="s">
         <v>721</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>729</v>
       </c>
       <c r="C8">
@@ -15415,7 +15507,7 @@
       <c r="A12" t="s">
         <v>722</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>730</v>
       </c>
       <c r="C12">

</xml_diff>

<commit_message>
Bigger K4 window size test
</commit_message>
<xml_diff>
--- a/Results/GO_DMGenes_woUPDOWN_0.01.xlsx
+++ b/Results/GO_DMGenes_woUPDOWN_0.01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19392" windowHeight="9168" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19392" windowHeight="9168" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="K4hU" sheetId="1" r:id="rId1"/>
@@ -2347,7 +2347,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2625,8 +2686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5107,6 +5168,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>1.5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5115,12 +5186,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="47.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7725,6 +7797,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>1.5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7733,8 +7815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10820,11 +10902,12 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D12" sqref="D12:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12007,8 +12090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B55" activeCellId="1" sqref="B60 B55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>